<commit_message>
fix: error about the user controller in message send success, update: add more test case in xlsx
</commit_message>
<xml_diff>
--- a/tests/Test-web.xlsx
+++ b/tests/Test-web.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Memory-D-space\xampp\htdocs\CourseWork\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62BD169-D2F2-4B3B-B945-C5B42D06E79D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B5CD31-CBE2-40F5-B5E6-E0FBE884894F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="12170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="11050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="409">
   <si>
     <r>
       <rPr>
@@ -1932,6 +1932,55 @@
     <t>ADMIN-2 2025-04-08 124218.png
 ADMIN-2 2025-04-08 122020.png
 ADMIN-2 2025-04-08 121853.png</t>
+  </si>
+  <si>
+    <t>SEND_EMAIL</t>
+  </si>
+  <si>
+    <t>User can send email to Admin by 
+Click to contact us and input the message into message box</t>
+  </si>
+  <si>
+    <t>1. Login
+2. Input message</t>
+  </si>
+  <si>
+    <t>23/4/2025</t>
+  </si>
+  <si>
+    <t>1 Message : Test send email 
+message</t>
+  </si>
+  <si>
+    <t>If it is successful, then will redirect 
+user to successful page and wait for 5 seconds before back the previous page</t>
+  </si>
+  <si>
+    <t>It redirect to successful page
+ and after 5 seconds back to previous page</t>
+  </si>
+  <si>
+    <t>SENDEMAIL-1-23-04-2025.png
+SENDEMAIL-1-b-23-04-2025.png
+SENDEMAIL-1-c-23-04-2025.png</t>
+  </si>
+  <si>
+    <t>ADMIN_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin can ban user </t>
+  </si>
+  <si>
+    <t>No input data</t>
+  </si>
+  <si>
+    <t>Admin can ban user by clicking to 
+ban button in user management page than that user account cannot use other features, only see the page forbidden message, and contact page</t>
+  </si>
+  <si>
+    <t>ADMIN-3-a 2025-04-23 191858.png
+ADMIN-3-b 2025-04-23 191915.png
+ADMIN-3-c 2025-04-23 191924.png</t>
   </si>
 </sst>
 </file>
@@ -2305,118 +2354,118 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2757,10 +2806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K76"/>
+  <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K74" activeCellId="1" sqref="J77 K74"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.3"/>
@@ -2810,16 +2859,16 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="52" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
     </row>
@@ -3002,25 +3051,25 @@
       <c r="J8" s="23"/>
     </row>
     <row r="9" spans="1:10" ht="98.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="36" t="s">
         <v>178</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="F9" s="41">
+      <c r="F9" s="37">
         <v>45842</v>
       </c>
-      <c r="G9" s="40" t="s">
+      <c r="G9" s="36" t="s">
         <v>182</v>
       </c>
       <c r="H9" s="14"/>
@@ -3032,25 +3081,25 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="140" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="36" t="s">
         <v>196</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="F10" s="41">
+      <c r="F10" s="37">
         <v>45842</v>
       </c>
-      <c r="G10" s="40" t="s">
+      <c r="G10" s="36" t="s">
         <v>96</v>
       </c>
       <c r="H10" s="14" t="s">
@@ -3062,62 +3111,62 @@
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" ht="140" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="45" t="s">
         <v>199</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="46" t="s">
         <v>193</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="46" t="s">
         <v>184</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="46" t="s">
         <v>194</v>
       </c>
-      <c r="E11" s="50" t="s">
+      <c r="E11" s="46" t="s">
         <v>195</v>
       </c>
-      <c r="F11" s="51">
+      <c r="F11" s="47">
         <v>45842</v>
       </c>
-      <c r="G11" s="50" t="s">
+      <c r="G11" s="46" t="s">
         <v>195</v>
       </c>
-      <c r="H11" s="52"/>
-      <c r="I11" s="53" t="s">
-        <v>90</v>
-      </c>
-      <c r="J11" s="53" t="s">
+      <c r="H11" s="48"/>
+      <c r="I11" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="J11" s="49" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="140" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="51" t="s">
         <v>200</v>
       </c>
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="51" t="s">
         <v>201</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="C12" s="51" t="s">
         <v>202</v>
       </c>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="51" t="s">
         <v>203</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="F12" s="43">
+      <c r="F12" s="39">
         <v>45842</v>
       </c>
-      <c r="G12" s="42" t="s">
+      <c r="G12" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="H12" s="56"/>
-      <c r="I12" s="57" t="s">
-        <v>90</v>
-      </c>
-      <c r="J12" s="57" t="s">
+      <c r="H12" s="52"/>
+      <c r="I12" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="J12" s="53" t="s">
         <v>205</v>
       </c>
     </row>
@@ -3125,22 +3174,22 @@
       <c r="A13" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="36" t="s">
         <v>208</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="36" t="s">
         <v>209</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="36" t="s">
         <v>210</v>
       </c>
-      <c r="F13" s="41">
+      <c r="F13" s="37">
         <v>45842</v>
       </c>
-      <c r="G13" s="40" t="s">
+      <c r="G13" s="36" t="s">
         <v>210</v>
       </c>
       <c r="H13" s="14"/>
@@ -3151,30 +3200,30 @@
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="108.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="77.5" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="F14" s="41">
+      <c r="F14" s="37">
         <v>45842</v>
       </c>
-      <c r="G14" s="40" t="s">
+      <c r="G14" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="H14" s="45"/>
-      <c r="I14" s="39" t="s">
+      <c r="H14" s="41"/>
+      <c r="I14" s="35" t="s">
         <v>90</v>
       </c>
       <c r="J14" s="13" t="s">
@@ -3182,18 +3231,18 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
     </row>
     <row r="16" spans="1:10" ht="107" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
@@ -3436,32 +3485,32 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="177" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="F24" s="34">
+      <c r="F24" s="32">
         <v>45842</v>
       </c>
-      <c r="G24" s="31" t="s">
+      <c r="G24" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="H24" s="35"/>
-      <c r="I24" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="J24" s="36" t="s">
+      <c r="H24" s="33"/>
+      <c r="I24" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="J24" s="34" t="s">
         <v>151</v>
       </c>
     </row>
@@ -3526,32 +3575,32 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="409.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="E27" s="28" t="s">
+      <c r="E27" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="F27" s="29">
+      <c r="F27" s="27">
         <v>45842</v>
       </c>
-      <c r="G27" s="28" t="s">
+      <c r="G27" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="H27" s="28"/>
-      <c r="I27" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="J27" s="30" t="s">
+      <c r="H27" s="26"/>
+      <c r="I27" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="J27" s="28" t="s">
         <v>154</v>
       </c>
     </row>
@@ -3705,7 +3754,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="77.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="62" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>136</v>
       </c>
@@ -3735,7 +3784,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="62" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="46.5" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>137</v>
       </c>
@@ -3855,25 +3904,25 @@
       <c r="A38" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="46" t="s">
+      <c r="C38" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="D38" s="46" t="s">
+      <c r="D38" s="42" t="s">
         <v>87</v>
       </c>
       <c r="E38" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="F38" s="47">
+      <c r="F38" s="43">
         <v>45812</v>
       </c>
-      <c r="G38" s="46" t="s">
+      <c r="G38" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="H38" s="48"/>
+      <c r="H38" s="44"/>
       <c r="I38" s="23" t="s">
         <v>90</v>
       </c>
@@ -3881,7 +3930,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="186" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="139.5" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>142</v>
       </c>
@@ -3912,18 +3961,18 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="59" t="s">
+      <c r="A40" s="61" t="s">
         <v>213</v>
       </c>
-      <c r="B40" s="58"/>
-      <c r="C40" s="58"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="58"/>
-      <c r="F40" s="58"/>
-      <c r="G40" s="58"/>
-      <c r="H40" s="58"/>
-      <c r="I40" s="58"/>
-      <c r="J40" s="58"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="62"/>
+      <c r="F40" s="62"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="62"/>
+      <c r="J40" s="62"/>
     </row>
     <row r="41" spans="1:10" ht="163" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
@@ -4260,35 +4309,35 @@
       </c>
     </row>
     <row r="52" spans="1:11" ht="170.5" x14ac:dyDescent="0.3">
-      <c r="A52" s="30" t="s">
+      <c r="A52" s="28" t="s">
         <v>271</v>
       </c>
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="C52" s="28" t="s">
+      <c r="C52" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="D52" s="28" t="s">
+      <c r="D52" s="26" t="s">
         <v>276</v>
       </c>
-      <c r="E52" s="28" t="s">
+      <c r="E52" s="26" t="s">
         <v>277</v>
       </c>
-      <c r="F52" s="29">
+      <c r="F52" s="27">
         <v>45873</v>
       </c>
-      <c r="G52" s="28" t="s">
+      <c r="G52" s="26" t="s">
         <v>277</v>
       </c>
-      <c r="H52" s="30"/>
-      <c r="I52" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="J52" s="30" t="s">
+      <c r="H52" s="28"/>
+      <c r="I52" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="J52" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="K52" s="54"/>
+      <c r="K52" s="50"/>
     </row>
     <row r="53" spans="1:11" ht="62" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
@@ -4364,7 +4413,9 @@
       <c r="E55" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="F55" s="13"/>
+      <c r="F55" s="15">
+        <v>45873</v>
+      </c>
       <c r="G55" s="14" t="s">
         <v>295</v>
       </c>
@@ -4392,7 +4443,9 @@
       <c r="E56" s="14" t="s">
         <v>299</v>
       </c>
-      <c r="F56" s="13"/>
+      <c r="F56" s="15">
+        <v>45873</v>
+      </c>
       <c r="G56" s="14" t="s">
         <v>300</v>
       </c>
@@ -4420,7 +4473,9 @@
       <c r="E57" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="F57" s="13"/>
+      <c r="F57" s="15">
+        <v>45873</v>
+      </c>
       <c r="G57" s="14" t="s">
         <v>277</v>
       </c>
@@ -4448,7 +4503,9 @@
       <c r="E58" s="14" t="s">
         <v>312</v>
       </c>
-      <c r="F58" s="13"/>
+      <c r="F58" s="15">
+        <v>45873</v>
+      </c>
       <c r="G58" s="14" t="s">
         <v>313</v>
       </c>
@@ -4476,7 +4533,9 @@
       <c r="E59" s="14" t="s">
         <v>319</v>
       </c>
-      <c r="F59" s="13"/>
+      <c r="F59" s="15">
+        <v>45873</v>
+      </c>
       <c r="G59" s="14" t="s">
         <v>321</v>
       </c>
@@ -4504,7 +4563,9 @@
       <c r="E60" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="F60" s="13"/>
+      <c r="F60" s="15">
+        <v>45873</v>
+      </c>
       <c r="G60" s="14" t="s">
         <v>326</v>
       </c>
@@ -4532,7 +4593,9 @@
       <c r="E61" s="14" t="s">
         <v>332</v>
       </c>
-      <c r="F61" s="13"/>
+      <c r="F61" s="15">
+        <v>45873</v>
+      </c>
       <c r="G61" s="14" t="s">
         <v>333</v>
       </c>
@@ -4545,18 +4608,18 @@
       </c>
     </row>
     <row r="62" spans="1:11" ht="33.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="60" t="s">
+      <c r="A62" s="54" t="s">
         <v>338</v>
       </c>
-      <c r="B62" s="61"/>
-      <c r="C62" s="61"/>
-      <c r="D62" s="61"/>
-      <c r="E62" s="61"/>
-      <c r="F62" s="61"/>
-      <c r="G62" s="61"/>
-      <c r="H62" s="61"/>
-      <c r="I62" s="61"/>
-      <c r="J62" s="62"/>
+      <c r="B62" s="55"/>
+      <c r="C62" s="55"/>
+      <c r="D62" s="55"/>
+      <c r="E62" s="55"/>
+      <c r="F62" s="55"/>
+      <c r="G62" s="55"/>
+      <c r="H62" s="55"/>
+      <c r="I62" s="55"/>
+      <c r="J62" s="56"/>
     </row>
     <row r="63" spans="1:11" ht="279" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
@@ -4574,7 +4637,9 @@
       <c r="E63" s="14" t="s">
         <v>340</v>
       </c>
-      <c r="F63" s="13"/>
+      <c r="F63" s="15">
+        <v>45873</v>
+      </c>
       <c r="G63" s="14" t="s">
         <v>341</v>
       </c>
@@ -4604,7 +4669,9 @@
       <c r="E64" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="F64" s="13"/>
+      <c r="F64" s="15">
+        <v>45873</v>
+      </c>
       <c r="G64" s="14" t="s">
         <v>349</v>
       </c>
@@ -4617,18 +4684,18 @@
       </c>
     </row>
     <row r="65" spans="1:10" ht="31" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="60" t="s">
+      <c r="A65" s="54" t="s">
         <v>350</v>
       </c>
-      <c r="B65" s="61"/>
-      <c r="C65" s="61"/>
-      <c r="D65" s="61"/>
-      <c r="E65" s="61"/>
-      <c r="F65" s="61"/>
-      <c r="G65" s="61"/>
-      <c r="H65" s="61"/>
-      <c r="I65" s="61"/>
-      <c r="J65" s="62"/>
+      <c r="B65" s="55"/>
+      <c r="C65" s="55"/>
+      <c r="D65" s="55"/>
+      <c r="E65" s="55"/>
+      <c r="F65" s="55"/>
+      <c r="G65" s="55"/>
+      <c r="H65" s="55"/>
+      <c r="I65" s="55"/>
+      <c r="J65" s="56"/>
     </row>
     <row r="66" spans="1:10" ht="77.5" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
@@ -4646,7 +4713,9 @@
       <c r="E66" s="14" t="s">
         <v>355</v>
       </c>
-      <c r="F66" s="13"/>
+      <c r="F66" s="15">
+        <v>45873</v>
+      </c>
       <c r="G66" s="14" t="s">
         <v>356</v>
       </c>
@@ -4659,18 +4728,18 @@
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" s="60" t="s">
+      <c r="A67" s="54" t="s">
         <v>358</v>
       </c>
-      <c r="B67" s="61"/>
-      <c r="C67" s="61"/>
-      <c r="D67" s="61"/>
-      <c r="E67" s="61"/>
-      <c r="F67" s="61"/>
-      <c r="G67" s="61"/>
-      <c r="H67" s="61"/>
-      <c r="I67" s="61"/>
-      <c r="J67" s="62"/>
+      <c r="B67" s="55"/>
+      <c r="C67" s="55"/>
+      <c r="D67" s="55"/>
+      <c r="E67" s="55"/>
+      <c r="F67" s="55"/>
+      <c r="G67" s="55"/>
+      <c r="H67" s="55"/>
+      <c r="I67" s="55"/>
+      <c r="J67" s="56"/>
     </row>
     <row r="68" spans="1:10" ht="139.5" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
@@ -4688,7 +4757,9 @@
       <c r="E68" s="14" t="s">
         <v>363</v>
       </c>
-      <c r="F68" s="13"/>
+      <c r="F68" s="15">
+        <v>45873</v>
+      </c>
       <c r="G68" s="13" t="s">
         <v>364</v>
       </c>
@@ -4716,7 +4787,9 @@
       <c r="E69" s="14" t="s">
         <v>363</v>
       </c>
-      <c r="F69" s="13"/>
+      <c r="F69" s="15">
+        <v>45873</v>
+      </c>
       <c r="G69" s="14" t="s">
         <v>380</v>
       </c>
@@ -4744,7 +4817,9 @@
       <c r="E70" s="14" t="s">
         <v>377</v>
       </c>
-      <c r="F70" s="13"/>
+      <c r="F70" s="15">
+        <v>45873</v>
+      </c>
       <c r="G70" s="14" t="s">
         <v>378</v>
       </c>
@@ -4772,7 +4847,9 @@
       <c r="E71" s="14" t="s">
         <v>369</v>
       </c>
-      <c r="F71" s="13"/>
+      <c r="F71" s="15">
+        <v>45873</v>
+      </c>
       <c r="G71" s="14" t="s">
         <v>369</v>
       </c>
@@ -4785,18 +4862,18 @@
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A72" s="60" t="s">
+      <c r="A72" s="54" t="s">
         <v>386</v>
       </c>
-      <c r="B72" s="61"/>
-      <c r="C72" s="61"/>
-      <c r="D72" s="61"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="61"/>
-      <c r="G72" s="61"/>
-      <c r="H72" s="61"/>
-      <c r="I72" s="61"/>
-      <c r="J72" s="62"/>
+      <c r="B72" s="55"/>
+      <c r="C72" s="55"/>
+      <c r="D72" s="55"/>
+      <c r="E72" s="55"/>
+      <c r="F72" s="55"/>
+      <c r="G72" s="55"/>
+      <c r="H72" s="55"/>
+      <c r="I72" s="55"/>
+      <c r="J72" s="56"/>
     </row>
     <row r="73" spans="1:10" ht="93" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
@@ -4814,7 +4891,9 @@
       <c r="E73" s="14" t="s">
         <v>384</v>
       </c>
-      <c r="F73" s="13"/>
+      <c r="F73" s="15">
+        <v>45873</v>
+      </c>
       <c r="G73" s="14" t="s">
         <v>385</v>
       </c>
@@ -4842,7 +4921,9 @@
       <c r="E74" s="14" t="s">
         <v>393</v>
       </c>
-      <c r="F74" s="13"/>
+      <c r="F74" s="15">
+        <v>45873</v>
+      </c>
       <c r="G74" s="14" t="s">
         <v>394</v>
       </c>
@@ -4854,29 +4935,77 @@
         <v>395</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A75" s="13"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="13"/>
-      <c r="F75" s="13"/>
-      <c r="G75" s="13"/>
+    <row r="75" spans="1:10" ht="232.5" x14ac:dyDescent="0.3">
+      <c r="A75" s="13" t="s">
+        <v>404</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>405</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="D75" s="13" t="s">
+        <v>406</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>407</v>
+      </c>
+      <c r="F75" s="13" t="s">
+        <v>399</v>
+      </c>
+      <c r="G75" s="14" t="s">
+        <v>407</v>
+      </c>
       <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="13"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A76" s="13"/>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
-      <c r="E76" s="13"/>
-      <c r="F76" s="13"/>
-      <c r="G76" s="13"/>
+      <c r="I75" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="J75" s="14" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="170.5" x14ac:dyDescent="0.3">
+      <c r="A76" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>398</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>400</v>
+      </c>
+      <c r="E76" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="F76" s="15" t="s">
+        <v>399</v>
+      </c>
+      <c r="G76" s="14" t="s">
+        <v>402</v>
+      </c>
       <c r="H76" s="13"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="13"/>
+      <c r="I76" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="J76" s="14" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="13"/>
+      <c r="B77" s="13"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>